<commit_message>
Updates to Satellite Sites
</commit_message>
<xml_diff>
--- a/Satellite Sites.xlsx
+++ b/Satellite Sites.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="361">
   <si>
     <t>Northwest</t>
   </si>
@@ -1560,6 +1560,198 @@
   </si>
   <si>
     <t>"http://weather.gc.ca/data/satellite/hrpt_ykn_nir_100.jpg"</t>
+  </si>
+  <si>
+    <t>Southern Ontario</t>
+  </si>
+  <si>
+    <r>
+      <t>"http://www.ssd.noaa.gov/goes/east/gl/img/" + "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YYYYDDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hhmmoption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.jpg"</t>
+    </r>
+  </si>
+  <si>
+    <t>Southern Quebec</t>
+  </si>
+  <si>
+    <t>Southern Western Canada</t>
+  </si>
+  <si>
+    <t>Southern Prairies</t>
+  </si>
+  <si>
+    <r>
+      <t>"http://www.ssd.noaa.gov/goes/east/ne/img/ + "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YYYYDDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hhmmoption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.jpg"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"http://www.ssd.noaa.gov/goes/east/np/img/ + "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YYYYDDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hhmmoption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.jpg"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"http://www.ssd.noaa.gov/goes/west/nw/img/ + "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YYYYDDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hhmmoption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.jpg"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1897,7 +2089,7 @@
   <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,10 +3590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3468,6 +3660,12 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="s">
+        <v>354</v>
+      </c>
       <c r="K6" t="s">
         <v>319</v>
       </c>
@@ -3475,110 +3673,135 @@
         <v>317</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" t="s">
+        <v>358</v>
+      </c>
+    </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>356</v>
+      </c>
+      <c r="B8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>333</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>341</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K10" t="s">
         <v>320</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K11" t="s">
         <v>319</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>331</v>
-      </c>
-      <c r="B12" t="s">
-        <v>340</v>
-      </c>
-      <c r="K12" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>337</v>
-      </c>
-      <c r="B15" t="s">
-        <v>339</v>
-      </c>
-      <c r="K15" t="s">
-        <v>320</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1070</v>
+        <v>331</v>
+      </c>
+      <c r="B14" t="s">
+        <v>340</v>
+      </c>
+      <c r="K14" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" t="s">
+        <v>339</v>
+      </c>
+      <c r="K17" t="s">
+        <v>320</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>346</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>349</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K18" t="s">
         <v>319</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>348</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>350</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K20" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>352</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K21" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
         <v>351</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>